<commit_message>
Uploading new pupae and fly data.
</commit_message>
<xml_diff>
--- a/data/fitness_development/MFE_flies.xlsx
+++ b/data/fitness_development/MFE_flies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_18/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7863335A-6F43-AB4B-BAB4-95E22CB8348C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7833B277-7CE6-B34B-B22A-134300AB292A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F87DAE63-E76D-134A-8567-557F4C2DF883}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="7">
   <si>
     <t>vial</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E795774-325B-7540-93CB-61EC9638DF3F}">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="82" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2428,6 +2428,493 @@
         <v>0</v>
       </c>
     </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>1</v>
+      </c>
+      <c r="B118" t="s">
+        <v>5</v>
+      </c>
+      <c r="C118">
+        <v>332</v>
+      </c>
+      <c r="D118">
+        <v>3</v>
+      </c>
+      <c r="E118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>1</v>
+      </c>
+      <c r="B119" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119">
+        <v>332</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>2</v>
+      </c>
+      <c r="B120" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120">
+        <v>332</v>
+      </c>
+      <c r="D120">
+        <v>5</v>
+      </c>
+      <c r="E120">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>2</v>
+      </c>
+      <c r="B121" t="s">
+        <v>6</v>
+      </c>
+      <c r="C121">
+        <v>332</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>3</v>
+      </c>
+      <c r="B122" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122">
+        <v>332</v>
+      </c>
+      <c r="D122">
+        <v>5</v>
+      </c>
+      <c r="E122">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>3</v>
+      </c>
+      <c r="B123" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123">
+        <v>332</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>4</v>
+      </c>
+      <c r="B124" t="s">
+        <v>5</v>
+      </c>
+      <c r="C124">
+        <v>332</v>
+      </c>
+      <c r="D124">
+        <v>5</v>
+      </c>
+      <c r="E124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>4</v>
+      </c>
+      <c r="B125" t="s">
+        <v>6</v>
+      </c>
+      <c r="C125">
+        <v>332</v>
+      </c>
+      <c r="D125">
+        <v>4</v>
+      </c>
+      <c r="E125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>5</v>
+      </c>
+      <c r="B126" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126">
+        <v>332</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>5</v>
+      </c>
+      <c r="B127" t="s">
+        <v>6</v>
+      </c>
+      <c r="C127">
+        <v>332</v>
+      </c>
+      <c r="D127">
+        <v>5</v>
+      </c>
+      <c r="E127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>6</v>
+      </c>
+      <c r="B128" t="s">
+        <v>5</v>
+      </c>
+      <c r="C128">
+        <v>332</v>
+      </c>
+      <c r="D128">
+        <v>2</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>6</v>
+      </c>
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129">
+        <v>332</v>
+      </c>
+      <c r="D129">
+        <v>4</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>7</v>
+      </c>
+      <c r="B130" t="s">
+        <v>5</v>
+      </c>
+      <c r="C130">
+        <v>332</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>7</v>
+      </c>
+      <c r="B131" t="s">
+        <v>6</v>
+      </c>
+      <c r="C131">
+        <v>332</v>
+      </c>
+      <c r="D131">
+        <v>4</v>
+      </c>
+      <c r="E131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>8</v>
+      </c>
+      <c r="B132" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132">
+        <v>332</v>
+      </c>
+      <c r="D132">
+        <v>3</v>
+      </c>
+      <c r="E132">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>8</v>
+      </c>
+      <c r="B133" t="s">
+        <v>6</v>
+      </c>
+      <c r="C133">
+        <v>332</v>
+      </c>
+      <c r="D133">
+        <v>3</v>
+      </c>
+      <c r="E133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>9</v>
+      </c>
+      <c r="B134" t="s">
+        <v>5</v>
+      </c>
+      <c r="C134">
+        <v>332</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>9</v>
+      </c>
+      <c r="B135" t="s">
+        <v>6</v>
+      </c>
+      <c r="C135">
+        <v>332</v>
+      </c>
+      <c r="D135">
+        <v>4</v>
+      </c>
+      <c r="E135">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>10</v>
+      </c>
+      <c r="B136" t="s">
+        <v>5</v>
+      </c>
+      <c r="C136">
+        <v>332</v>
+      </c>
+      <c r="D136">
+        <v>4</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>10</v>
+      </c>
+      <c r="B137" t="s">
+        <v>6</v>
+      </c>
+      <c r="C137">
+        <v>332</v>
+      </c>
+      <c r="D137">
+        <v>8</v>
+      </c>
+      <c r="E137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>11</v>
+      </c>
+      <c r="B138" t="s">
+        <v>5</v>
+      </c>
+      <c r="C138">
+        <v>332</v>
+      </c>
+      <c r="D138">
+        <v>3</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>11</v>
+      </c>
+      <c r="B139" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139">
+        <v>332</v>
+      </c>
+      <c r="D139">
+        <v>3</v>
+      </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>12</v>
+      </c>
+      <c r="B140" t="s">
+        <v>5</v>
+      </c>
+      <c r="C140">
+        <v>332</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>12</v>
+      </c>
+      <c r="B141" t="s">
+        <v>6</v>
+      </c>
+      <c r="C141">
+        <v>332</v>
+      </c>
+      <c r="D141">
+        <v>4</v>
+      </c>
+      <c r="E141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>13</v>
+      </c>
+      <c r="B142" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142">
+        <v>332</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>13</v>
+      </c>
+      <c r="B143" t="s">
+        <v>6</v>
+      </c>
+      <c r="C143">
+        <v>332</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>14</v>
+      </c>
+      <c r="B144" t="s">
+        <v>5</v>
+      </c>
+      <c r="C144">
+        <v>332</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>14</v>
+      </c>
+      <c r="B145" t="s">
+        <v>6</v>
+      </c>
+      <c r="C145">
+        <v>332</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>15</v>
+      </c>
+      <c r="B146" t="s">
+        <v>6</v>
+      </c>
+      <c r="C146">
+        <v>332</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating fly and pupae data.
</commit_message>
<xml_diff>
--- a/data/fitness_development/MFE_flies.xlsx
+++ b/data/fitness_development/MFE_flies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_18/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7833B277-7CE6-B34B-B22A-134300AB292A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{84FEE38E-FE6E-2445-971C-1456B84EA9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F87DAE63-E76D-134A-8567-557F4C2DF883}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{F87DAE63-E76D-134A-8567-557F4C2DF883}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="7">
   <si>
     <t>vial</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E795774-325B-7540-93CB-61EC9638DF3F}">
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="82" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D146" sqref="D146"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="82" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F204" sqref="F204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2914,6 +2914,998 @@
       <c r="C146">
         <v>332</v>
       </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>1</v>
+      </c>
+      <c r="B147" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147">
+        <v>341</v>
+      </c>
+      <c r="D147">
+        <v>6</v>
+      </c>
+      <c r="E147">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>1</v>
+      </c>
+      <c r="B148" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148">
+        <v>341</v>
+      </c>
+      <c r="D148">
+        <v>0</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>2</v>
+      </c>
+      <c r="B149" t="s">
+        <v>5</v>
+      </c>
+      <c r="C149">
+        <v>341</v>
+      </c>
+      <c r="D149">
+        <v>3</v>
+      </c>
+      <c r="E149">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>2</v>
+      </c>
+      <c r="B150" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150">
+        <v>341</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>3</v>
+      </c>
+      <c r="B151" t="s">
+        <v>5</v>
+      </c>
+      <c r="C151">
+        <v>341</v>
+      </c>
+      <c r="D151">
+        <v>3</v>
+      </c>
+      <c r="E151">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>3</v>
+      </c>
+      <c r="B152" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152">
+        <v>341</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>4</v>
+      </c>
+      <c r="B153" t="s">
+        <v>5</v>
+      </c>
+      <c r="C153">
+        <v>341</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+      <c r="E153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>4</v>
+      </c>
+      <c r="B154" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154">
+        <v>341</v>
+      </c>
+      <c r="D154">
+        <v>3</v>
+      </c>
+      <c r="E154">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>5</v>
+      </c>
+      <c r="B155" t="s">
+        <v>5</v>
+      </c>
+      <c r="C155">
+        <v>341</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>5</v>
+      </c>
+      <c r="B156" t="s">
+        <v>6</v>
+      </c>
+      <c r="C156">
+        <v>341</v>
+      </c>
+      <c r="D156">
+        <v>5</v>
+      </c>
+      <c r="E156">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>6</v>
+      </c>
+      <c r="B157" t="s">
+        <v>5</v>
+      </c>
+      <c r="C157">
+        <v>341</v>
+      </c>
+      <c r="D157">
+        <v>5</v>
+      </c>
+      <c r="E157">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>6</v>
+      </c>
+      <c r="B158" t="s">
+        <v>6</v>
+      </c>
+      <c r="C158">
+        <v>341</v>
+      </c>
+      <c r="D158">
+        <v>2</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>7</v>
+      </c>
+      <c r="B159" t="s">
+        <v>5</v>
+      </c>
+      <c r="C159">
+        <v>341</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>7</v>
+      </c>
+      <c r="B160" t="s">
+        <v>6</v>
+      </c>
+      <c r="C160">
+        <v>341</v>
+      </c>
+      <c r="D160">
+        <v>7</v>
+      </c>
+      <c r="E160">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>8</v>
+      </c>
+      <c r="B161" t="s">
+        <v>5</v>
+      </c>
+      <c r="C161">
+        <v>341</v>
+      </c>
+      <c r="D161">
+        <v>4</v>
+      </c>
+      <c r="E161">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>8</v>
+      </c>
+      <c r="B162" t="s">
+        <v>6</v>
+      </c>
+      <c r="C162">
+        <v>341</v>
+      </c>
+      <c r="D162">
+        <v>6</v>
+      </c>
+      <c r="E162">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>9</v>
+      </c>
+      <c r="B163" t="s">
+        <v>5</v>
+      </c>
+      <c r="C163">
+        <v>341</v>
+      </c>
+      <c r="D163">
+        <v>2</v>
+      </c>
+      <c r="E163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>9</v>
+      </c>
+      <c r="B164" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164">
+        <v>341</v>
+      </c>
+      <c r="D164">
+        <v>5</v>
+      </c>
+      <c r="E164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>10</v>
+      </c>
+      <c r="B165" t="s">
+        <v>5</v>
+      </c>
+      <c r="C165">
+        <v>341</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>10</v>
+      </c>
+      <c r="B166" t="s">
+        <v>6</v>
+      </c>
+      <c r="C166">
+        <v>341</v>
+      </c>
+      <c r="D166">
+        <v>3</v>
+      </c>
+      <c r="E166">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>11</v>
+      </c>
+      <c r="B167" t="s">
+        <v>5</v>
+      </c>
+      <c r="C167">
+        <v>341</v>
+      </c>
+      <c r="D167">
+        <v>3</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>11</v>
+      </c>
+      <c r="B168" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168">
+        <v>341</v>
+      </c>
+      <c r="D168">
+        <v>4</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>12</v>
+      </c>
+      <c r="B169" t="s">
+        <v>5</v>
+      </c>
+      <c r="C169">
+        <v>341</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="E169">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>12</v>
+      </c>
+      <c r="B170" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170">
+        <v>341</v>
+      </c>
+      <c r="D170">
+        <v>6</v>
+      </c>
+      <c r="E170">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>13</v>
+      </c>
+      <c r="B171" t="s">
+        <v>5</v>
+      </c>
+      <c r="C171">
+        <v>341</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>13</v>
+      </c>
+      <c r="B172" t="s">
+        <v>6</v>
+      </c>
+      <c r="C172">
+        <v>341</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="E172">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>14</v>
+      </c>
+      <c r="B173" t="s">
+        <v>5</v>
+      </c>
+      <c r="C173">
+        <v>341</v>
+      </c>
+      <c r="D173">
+        <v>4</v>
+      </c>
+      <c r="E173">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>14</v>
+      </c>
+      <c r="B174" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174">
+        <v>341</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>15</v>
+      </c>
+      <c r="B175" t="s">
+        <v>6</v>
+      </c>
+      <c r="C175">
+        <v>341</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+      <c r="E175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>1</v>
+      </c>
+      <c r="B176" t="s">
+        <v>5</v>
+      </c>
+      <c r="C176">
+        <v>356</v>
+      </c>
+      <c r="D176">
+        <v>0</v>
+      </c>
+      <c r="E176">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>1</v>
+      </c>
+      <c r="B177" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177">
+        <v>356</v>
+      </c>
+      <c r="D177">
+        <v>0</v>
+      </c>
+      <c r="E177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>2</v>
+      </c>
+      <c r="B178" t="s">
+        <v>5</v>
+      </c>
+      <c r="C178">
+        <v>356</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>2</v>
+      </c>
+      <c r="B179" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179">
+        <v>356</v>
+      </c>
+      <c r="D179">
+        <v>0</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>3</v>
+      </c>
+      <c r="B180" t="s">
+        <v>5</v>
+      </c>
+      <c r="C180">
+        <v>356</v>
+      </c>
+      <c r="D180">
+        <v>1</v>
+      </c>
+      <c r="E180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>3</v>
+      </c>
+      <c r="B181" t="s">
+        <v>6</v>
+      </c>
+      <c r="C181">
+        <v>356</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+      <c r="E181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>4</v>
+      </c>
+      <c r="B182" t="s">
+        <v>5</v>
+      </c>
+      <c r="C182">
+        <v>356</v>
+      </c>
+      <c r="D182">
+        <v>4</v>
+      </c>
+      <c r="E182">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>4</v>
+      </c>
+      <c r="B183" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183">
+        <v>356</v>
+      </c>
+      <c r="D183">
+        <v>2</v>
+      </c>
+      <c r="E183">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>5</v>
+      </c>
+      <c r="B184" t="s">
+        <v>5</v>
+      </c>
+      <c r="C184">
+        <v>356</v>
+      </c>
+      <c r="D184">
+        <v>1</v>
+      </c>
+      <c r="E184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>5</v>
+      </c>
+      <c r="B185" t="s">
+        <v>6</v>
+      </c>
+      <c r="C185">
+        <v>356</v>
+      </c>
+      <c r="D185">
+        <v>3</v>
+      </c>
+      <c r="E185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>6</v>
+      </c>
+      <c r="B186" t="s">
+        <v>5</v>
+      </c>
+      <c r="C186">
+        <v>356</v>
+      </c>
+      <c r="D186">
+        <v>1</v>
+      </c>
+      <c r="E186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>6</v>
+      </c>
+      <c r="B187" t="s">
+        <v>6</v>
+      </c>
+      <c r="C187">
+        <v>356</v>
+      </c>
+      <c r="D187">
+        <v>4</v>
+      </c>
+      <c r="E187">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>7</v>
+      </c>
+      <c r="B188" t="s">
+        <v>5</v>
+      </c>
+      <c r="C188">
+        <v>356</v>
+      </c>
+      <c r="D188">
+        <v>0</v>
+      </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>7</v>
+      </c>
+      <c r="B189" t="s">
+        <v>6</v>
+      </c>
+      <c r="C189">
+        <v>356</v>
+      </c>
+      <c r="D189">
+        <v>4</v>
+      </c>
+      <c r="E189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>8</v>
+      </c>
+      <c r="B190" t="s">
+        <v>5</v>
+      </c>
+      <c r="C190">
+        <v>356</v>
+      </c>
+      <c r="D190">
+        <v>3</v>
+      </c>
+      <c r="E190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>8</v>
+      </c>
+      <c r="B191" t="s">
+        <v>6</v>
+      </c>
+      <c r="C191">
+        <v>356</v>
+      </c>
+      <c r="D191">
+        <v>0</v>
+      </c>
+      <c r="E191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>9</v>
+      </c>
+      <c r="B192" t="s">
+        <v>5</v>
+      </c>
+      <c r="C192">
+        <v>356</v>
+      </c>
+      <c r="D192">
+        <v>1</v>
+      </c>
+      <c r="E192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>9</v>
+      </c>
+      <c r="B193" t="s">
+        <v>6</v>
+      </c>
+      <c r="C193">
+        <v>356</v>
+      </c>
+      <c r="D193">
+        <v>1</v>
+      </c>
+      <c r="E193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>10</v>
+      </c>
+      <c r="B194" t="s">
+        <v>5</v>
+      </c>
+      <c r="C194">
+        <v>356</v>
+      </c>
+      <c r="D194">
+        <v>0</v>
+      </c>
+      <c r="E194">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>10</v>
+      </c>
+      <c r="B195" t="s">
+        <v>6</v>
+      </c>
+      <c r="C195">
+        <v>356</v>
+      </c>
+      <c r="D195">
+        <v>2</v>
+      </c>
+      <c r="E195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>11</v>
+      </c>
+      <c r="B196" t="s">
+        <v>5</v>
+      </c>
+      <c r="C196">
+        <v>356</v>
+      </c>
+      <c r="D196">
+        <v>1</v>
+      </c>
+      <c r="E196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>11</v>
+      </c>
+      <c r="B197" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197">
+        <v>356</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+      <c r="E197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>12</v>
+      </c>
+      <c r="B198" t="s">
+        <v>5</v>
+      </c>
+      <c r="C198">
+        <v>356</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>12</v>
+      </c>
+      <c r="B199" t="s">
+        <v>6</v>
+      </c>
+      <c r="C199">
+        <v>356</v>
+      </c>
+      <c r="D199">
+        <v>1</v>
+      </c>
+      <c r="E199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>13</v>
+      </c>
+      <c r="B200" t="s">
+        <v>5</v>
+      </c>
+      <c r="C200">
+        <v>356</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>13</v>
+      </c>
+      <c r="B201" t="s">
+        <v>6</v>
+      </c>
+      <c r="C201">
+        <v>356</v>
+      </c>
+      <c r="D201">
+        <v>1</v>
+      </c>
+      <c r="E201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>14</v>
+      </c>
+      <c r="B202" t="s">
+        <v>5</v>
+      </c>
+      <c r="C202">
+        <v>356</v>
+      </c>
+      <c r="D202">
+        <v>2</v>
+      </c>
+      <c r="E202">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>14</v>
+      </c>
+      <c r="B203" t="s">
+        <v>6</v>
+      </c>
+      <c r="C203">
+        <v>356</v>
+      </c>
+      <c r="D203">
+        <v>0</v>
+      </c>
+      <c r="E203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>15</v>
+      </c>
+      <c r="B204" t="s">
+        <v>6</v>
+      </c>
+      <c r="C204">
+        <v>356</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="E204">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating fly and pupa data.
</commit_message>
<xml_diff>
--- a/data/fitness_development/MFE_flies.xlsx
+++ b/data/fitness_development/MFE_flies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_18/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84FEE38E-FE6E-2445-971C-1456B84EA9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69C76F9D-6EF2-1842-93FD-AD27AAEF107D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{F87DAE63-E76D-134A-8567-557F4C2DF883}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F87DAE63-E76D-134A-8567-557F4C2DF883}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="7">
   <si>
     <t>vial</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E795774-325B-7540-93CB-61EC9638DF3F}">
-  <dimension ref="A1:E204"/>
+  <dimension ref="A1:E233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="82" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F204" sqref="F204"/>
+    <sheetView tabSelected="1" topLeftCell="A218" zoomScale="161" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E233" sqref="E233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2966,10 +2966,10 @@
         <v>341</v>
       </c>
       <c r="D149">
+        <v>8</v>
+      </c>
+      <c r="E149">
         <v>3</v>
-      </c>
-      <c r="E149">
-        <v>8</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -3000,10 +3000,10 @@
         <v>341</v>
       </c>
       <c r="D151">
+        <v>4</v>
+      </c>
+      <c r="E151">
         <v>3</v>
-      </c>
-      <c r="E151">
-        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -3034,10 +3034,10 @@
         <v>341</v>
       </c>
       <c r="D153">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E153">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -3051,10 +3051,10 @@
         <v>341</v>
       </c>
       <c r="D154">
+        <v>4</v>
+      </c>
+      <c r="E154">
         <v>3</v>
-      </c>
-      <c r="E154">
-        <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -3085,10 +3085,10 @@
         <v>341</v>
       </c>
       <c r="D156">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E156">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -3102,10 +3102,10 @@
         <v>341</v>
       </c>
       <c r="D157">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E157">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -3119,10 +3119,10 @@
         <v>341</v>
       </c>
       <c r="D158">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E158">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -3153,10 +3153,10 @@
         <v>341</v>
       </c>
       <c r="D160">
+        <v>3</v>
+      </c>
+      <c r="E160">
         <v>7</v>
-      </c>
-      <c r="E160">
-        <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
@@ -3170,10 +3170,10 @@
         <v>341</v>
       </c>
       <c r="D161">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E161">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -3187,10 +3187,10 @@
         <v>341</v>
       </c>
       <c r="D162">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E162">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -3221,10 +3221,10 @@
         <v>341</v>
       </c>
       <c r="D164">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E164">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -3238,10 +3238,10 @@
         <v>341</v>
       </c>
       <c r="D165">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E165">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -3255,10 +3255,10 @@
         <v>341</v>
       </c>
       <c r="D166">
+        <v>4</v>
+      </c>
+      <c r="E166">
         <v>3</v>
-      </c>
-      <c r="E166">
-        <v>4</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -3272,10 +3272,10 @@
         <v>341</v>
       </c>
       <c r="D167">
+        <v>1</v>
+      </c>
+      <c r="E167">
         <v>3</v>
-      </c>
-      <c r="E167">
-        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -3289,10 +3289,10 @@
         <v>341</v>
       </c>
       <c r="D168">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E168">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
@@ -3306,10 +3306,10 @@
         <v>341</v>
       </c>
       <c r="D169">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E169">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -3323,10 +3323,10 @@
         <v>341</v>
       </c>
       <c r="D170">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E170">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -3357,10 +3357,10 @@
         <v>341</v>
       </c>
       <c r="D172">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E172">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -3374,10 +3374,10 @@
         <v>341</v>
       </c>
       <c r="D173">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E173">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -3408,10 +3408,10 @@
         <v>341</v>
       </c>
       <c r="D175">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E175">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -3425,10 +3425,10 @@
         <v>356</v>
       </c>
       <c r="D176">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E176">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -3459,10 +3459,10 @@
         <v>356</v>
       </c>
       <c r="D178">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E178">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
@@ -3544,10 +3544,10 @@
         <v>356</v>
       </c>
       <c r="D183">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E183">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -3561,10 +3561,10 @@
         <v>356</v>
       </c>
       <c r="D184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E184">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
@@ -3578,10 +3578,10 @@
         <v>356</v>
       </c>
       <c r="D185">
+        <v>0</v>
+      </c>
+      <c r="E185">
         <v>3</v>
-      </c>
-      <c r="E185">
-        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
@@ -3612,10 +3612,10 @@
         <v>356</v>
       </c>
       <c r="D187">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E187">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
@@ -3646,10 +3646,10 @@
         <v>356</v>
       </c>
       <c r="D189">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E189">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
@@ -3663,10 +3663,10 @@
         <v>356</v>
       </c>
       <c r="D190">
+        <v>1</v>
+      </c>
+      <c r="E190">
         <v>3</v>
-      </c>
-      <c r="E190">
-        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
@@ -3680,10 +3680,10 @@
         <v>356</v>
       </c>
       <c r="D191">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E191">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -3714,10 +3714,10 @@
         <v>356</v>
       </c>
       <c r="D193">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E193">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -3731,10 +3731,10 @@
         <v>356</v>
       </c>
       <c r="D194">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E194">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -3799,10 +3799,10 @@
         <v>356</v>
       </c>
       <c r="D198">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E198">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
@@ -3816,10 +3816,10 @@
         <v>356</v>
       </c>
       <c r="D199">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E199">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
@@ -3905,6 +3905,499 @@
       </c>
       <c r="E204">
         <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>1</v>
+      </c>
+      <c r="B205" t="s">
+        <v>5</v>
+      </c>
+      <c r="C205">
+        <v>365</v>
+      </c>
+      <c r="D205">
+        <v>1</v>
+      </c>
+      <c r="E205">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>1</v>
+      </c>
+      <c r="B206" t="s">
+        <v>6</v>
+      </c>
+      <c r="C206">
+        <v>365</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>2</v>
+      </c>
+      <c r="B207" t="s">
+        <v>5</v>
+      </c>
+      <c r="C207">
+        <v>365</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+      <c r="E207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>2</v>
+      </c>
+      <c r="B208" t="s">
+        <v>6</v>
+      </c>
+      <c r="C208">
+        <v>365</v>
+      </c>
+      <c r="D208">
+        <v>0</v>
+      </c>
+      <c r="E208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>3</v>
+      </c>
+      <c r="B209" t="s">
+        <v>5</v>
+      </c>
+      <c r="C209">
+        <v>365</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>3</v>
+      </c>
+      <c r="B210" t="s">
+        <v>6</v>
+      </c>
+      <c r="C210">
+        <v>365</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>4</v>
+      </c>
+      <c r="B211" t="s">
+        <v>5</v>
+      </c>
+      <c r="C211">
+        <v>365</v>
+      </c>
+      <c r="D211">
+        <v>1</v>
+      </c>
+      <c r="E211">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>4</v>
+      </c>
+      <c r="B212" t="s">
+        <v>6</v>
+      </c>
+      <c r="C212">
+        <v>365</v>
+      </c>
+      <c r="D212">
+        <v>6</v>
+      </c>
+      <c r="E212">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>5</v>
+      </c>
+      <c r="B213" t="s">
+        <v>5</v>
+      </c>
+      <c r="C213">
+        <v>365</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+      <c r="E213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>5</v>
+      </c>
+      <c r="B214" t="s">
+        <v>6</v>
+      </c>
+      <c r="C214">
+        <v>365</v>
+      </c>
+      <c r="D214">
+        <v>3</v>
+      </c>
+      <c r="E214">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>6</v>
+      </c>
+      <c r="B215" t="s">
+        <v>5</v>
+      </c>
+      <c r="C215">
+        <v>365</v>
+      </c>
+      <c r="D215">
+        <v>2</v>
+      </c>
+      <c r="E215">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>6</v>
+      </c>
+      <c r="B216" t="s">
+        <v>6</v>
+      </c>
+      <c r="C216">
+        <v>365</v>
+      </c>
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>7</v>
+      </c>
+      <c r="B217" t="s">
+        <v>5</v>
+      </c>
+      <c r="C217">
+        <v>365</v>
+      </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>7</v>
+      </c>
+      <c r="B218" t="s">
+        <v>6</v>
+      </c>
+      <c r="C218">
+        <v>365</v>
+      </c>
+      <c r="D218">
+        <v>3</v>
+      </c>
+      <c r="E218">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>8</v>
+      </c>
+      <c r="B219" t="s">
+        <v>5</v>
+      </c>
+      <c r="C219">
+        <v>365</v>
+      </c>
+      <c r="D219">
+        <v>4</v>
+      </c>
+      <c r="E219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>8</v>
+      </c>
+      <c r="B220" t="s">
+        <v>6</v>
+      </c>
+      <c r="C220">
+        <v>365</v>
+      </c>
+      <c r="D220">
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>9</v>
+      </c>
+      <c r="B221" t="s">
+        <v>5</v>
+      </c>
+      <c r="C221">
+        <v>365</v>
+      </c>
+      <c r="D221">
+        <v>4</v>
+      </c>
+      <c r="E221">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>9</v>
+      </c>
+      <c r="B222" t="s">
+        <v>6</v>
+      </c>
+      <c r="C222">
+        <v>365</v>
+      </c>
+      <c r="D222">
+        <v>1</v>
+      </c>
+      <c r="E222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>10</v>
+      </c>
+      <c r="B223" t="s">
+        <v>5</v>
+      </c>
+      <c r="C223">
+        <v>365</v>
+      </c>
+      <c r="D223">
+        <v>4</v>
+      </c>
+      <c r="E223">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>10</v>
+      </c>
+      <c r="B224" t="s">
+        <v>6</v>
+      </c>
+      <c r="C224">
+        <v>365</v>
+      </c>
+      <c r="D224">
+        <v>4</v>
+      </c>
+      <c r="E224">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>11</v>
+      </c>
+      <c r="B225" t="s">
+        <v>5</v>
+      </c>
+      <c r="C225">
+        <v>365</v>
+      </c>
+      <c r="D225">
+        <v>2</v>
+      </c>
+      <c r="E225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>11</v>
+      </c>
+      <c r="B226" t="s">
+        <v>6</v>
+      </c>
+      <c r="C226">
+        <v>365</v>
+      </c>
+      <c r="D226">
+        <v>0</v>
+      </c>
+      <c r="E226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>12</v>
+      </c>
+      <c r="B227" t="s">
+        <v>5</v>
+      </c>
+      <c r="C227">
+        <v>365</v>
+      </c>
+      <c r="D227">
+        <v>0</v>
+      </c>
+      <c r="E227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>12</v>
+      </c>
+      <c r="B228" t="s">
+        <v>6</v>
+      </c>
+      <c r="C228">
+        <v>365</v>
+      </c>
+      <c r="D228">
+        <v>1</v>
+      </c>
+      <c r="E228">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>13</v>
+      </c>
+      <c r="B229" t="s">
+        <v>5</v>
+      </c>
+      <c r="C229">
+        <v>365</v>
+      </c>
+      <c r="D229">
+        <v>0</v>
+      </c>
+      <c r="E229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>13</v>
+      </c>
+      <c r="B230" t="s">
+        <v>6</v>
+      </c>
+      <c r="C230">
+        <v>365</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
+      <c r="E230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>14</v>
+      </c>
+      <c r="B231" t="s">
+        <v>5</v>
+      </c>
+      <c r="C231">
+        <v>365</v>
+      </c>
+      <c r="D231">
+        <v>3</v>
+      </c>
+      <c r="E231">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>14</v>
+      </c>
+      <c r="B232" t="s">
+        <v>6</v>
+      </c>
+      <c r="C232">
+        <v>365</v>
+      </c>
+      <c r="D232">
+        <v>0</v>
+      </c>
+      <c r="E232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>15</v>
+      </c>
+      <c r="B233" t="s">
+        <v>6</v>
+      </c>
+      <c r="C233">
+        <v>365</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+      <c r="E233">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding updated MFE data.
</commit_message>
<xml_diff>
--- a/data/fitness_development/MFE_flies.xlsx
+++ b/data/fitness_development/MFE_flies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_18/data/fitness_development/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_19/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69C76F9D-6EF2-1842-93FD-AD27AAEF107D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{60076FF9-E0C7-5343-BDF2-38F0F945FE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F87DAE63-E76D-134A-8567-557F4C2DF883}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="7">
   <si>
     <t>vial</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E795774-325B-7540-93CB-61EC9638DF3F}">
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:E320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" zoomScale="161" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E233" sqref="E233"/>
+    <sheetView tabSelected="1" topLeftCell="A284" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D293" sqref="D293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4400,6 +4400,1485 @@
         <v>1</v>
       </c>
     </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>1</v>
+      </c>
+      <c r="B234" t="s">
+        <v>5</v>
+      </c>
+      <c r="C234">
+        <v>380</v>
+      </c>
+      <c r="D234">
+        <v>2</v>
+      </c>
+      <c r="E234">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>1</v>
+      </c>
+      <c r="B235" t="s">
+        <v>6</v>
+      </c>
+      <c r="C235">
+        <v>380</v>
+      </c>
+      <c r="D235">
+        <v>0</v>
+      </c>
+      <c r="E235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>2</v>
+      </c>
+      <c r="B236" t="s">
+        <v>5</v>
+      </c>
+      <c r="C236">
+        <v>380</v>
+      </c>
+      <c r="D236">
+        <v>0</v>
+      </c>
+      <c r="E236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>2</v>
+      </c>
+      <c r="B237" t="s">
+        <v>6</v>
+      </c>
+      <c r="C237">
+        <v>380</v>
+      </c>
+      <c r="D237">
+        <v>0</v>
+      </c>
+      <c r="E237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>3</v>
+      </c>
+      <c r="B238" t="s">
+        <v>5</v>
+      </c>
+      <c r="C238">
+        <v>380</v>
+      </c>
+      <c r="D238">
+        <v>0</v>
+      </c>
+      <c r="E238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>3</v>
+      </c>
+      <c r="B239" t="s">
+        <v>6</v>
+      </c>
+      <c r="C239">
+        <v>380</v>
+      </c>
+      <c r="D239">
+        <v>0</v>
+      </c>
+      <c r="E239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>4</v>
+      </c>
+      <c r="B240" t="s">
+        <v>5</v>
+      </c>
+      <c r="C240">
+        <v>380</v>
+      </c>
+      <c r="D240">
+        <v>0</v>
+      </c>
+      <c r="E240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>4</v>
+      </c>
+      <c r="B241" t="s">
+        <v>6</v>
+      </c>
+      <c r="C241">
+        <v>380</v>
+      </c>
+      <c r="D241">
+        <v>2</v>
+      </c>
+      <c r="E241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>5</v>
+      </c>
+      <c r="B242" t="s">
+        <v>5</v>
+      </c>
+      <c r="C242">
+        <v>380</v>
+      </c>
+      <c r="D242">
+        <v>0</v>
+      </c>
+      <c r="E242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>5</v>
+      </c>
+      <c r="B243" t="s">
+        <v>6</v>
+      </c>
+      <c r="C243">
+        <v>380</v>
+      </c>
+      <c r="D243">
+        <v>0</v>
+      </c>
+      <c r="E243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>6</v>
+      </c>
+      <c r="B244" t="s">
+        <v>5</v>
+      </c>
+      <c r="C244">
+        <v>380</v>
+      </c>
+      <c r="D244">
+        <v>2</v>
+      </c>
+      <c r="E244">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>6</v>
+      </c>
+      <c r="B245" t="s">
+        <v>6</v>
+      </c>
+      <c r="C245">
+        <v>380</v>
+      </c>
+      <c r="D245">
+        <v>1</v>
+      </c>
+      <c r="E245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>7</v>
+      </c>
+      <c r="B246" t="s">
+        <v>5</v>
+      </c>
+      <c r="C246">
+        <v>380</v>
+      </c>
+      <c r="D246">
+        <v>0</v>
+      </c>
+      <c r="E246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>7</v>
+      </c>
+      <c r="B247" t="s">
+        <v>6</v>
+      </c>
+      <c r="C247">
+        <v>380</v>
+      </c>
+      <c r="D247">
+        <v>3</v>
+      </c>
+      <c r="E247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>8</v>
+      </c>
+      <c r="B248" t="s">
+        <v>5</v>
+      </c>
+      <c r="C248">
+        <v>380</v>
+      </c>
+      <c r="D248">
+        <v>0</v>
+      </c>
+      <c r="E248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>8</v>
+      </c>
+      <c r="B249" t="s">
+        <v>6</v>
+      </c>
+      <c r="C249">
+        <v>380</v>
+      </c>
+      <c r="D249">
+        <v>1</v>
+      </c>
+      <c r="E249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>9</v>
+      </c>
+      <c r="B250" t="s">
+        <v>5</v>
+      </c>
+      <c r="C250">
+        <v>380</v>
+      </c>
+      <c r="D250">
+        <v>0</v>
+      </c>
+      <c r="E250">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>9</v>
+      </c>
+      <c r="B251" t="s">
+        <v>6</v>
+      </c>
+      <c r="C251">
+        <v>380</v>
+      </c>
+      <c r="D251">
+        <v>0</v>
+      </c>
+      <c r="E251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>10</v>
+      </c>
+      <c r="B252" t="s">
+        <v>5</v>
+      </c>
+      <c r="C252">
+        <v>380</v>
+      </c>
+      <c r="D252">
+        <v>0</v>
+      </c>
+      <c r="E252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>10</v>
+      </c>
+      <c r="B253" t="s">
+        <v>6</v>
+      </c>
+      <c r="C253">
+        <v>380</v>
+      </c>
+      <c r="D253">
+        <v>1</v>
+      </c>
+      <c r="E253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>11</v>
+      </c>
+      <c r="B254" t="s">
+        <v>5</v>
+      </c>
+      <c r="C254">
+        <v>380</v>
+      </c>
+      <c r="D254">
+        <v>0</v>
+      </c>
+      <c r="E254">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>11</v>
+      </c>
+      <c r="B255" t="s">
+        <v>6</v>
+      </c>
+      <c r="C255">
+        <v>380</v>
+      </c>
+      <c r="D255">
+        <v>0</v>
+      </c>
+      <c r="E255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>12</v>
+      </c>
+      <c r="B256" t="s">
+        <v>5</v>
+      </c>
+      <c r="C256">
+        <v>380</v>
+      </c>
+      <c r="D256">
+        <v>0</v>
+      </c>
+      <c r="E256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>12</v>
+      </c>
+      <c r="B257" t="s">
+        <v>6</v>
+      </c>
+      <c r="C257">
+        <v>380</v>
+      </c>
+      <c r="D257">
+        <v>0</v>
+      </c>
+      <c r="E257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>13</v>
+      </c>
+      <c r="B258" t="s">
+        <v>5</v>
+      </c>
+      <c r="C258">
+        <v>380</v>
+      </c>
+      <c r="D258">
+        <v>0</v>
+      </c>
+      <c r="E258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>13</v>
+      </c>
+      <c r="B259" t="s">
+        <v>6</v>
+      </c>
+      <c r="C259">
+        <v>380</v>
+      </c>
+      <c r="D259">
+        <v>1</v>
+      </c>
+      <c r="E259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>14</v>
+      </c>
+      <c r="B260" t="s">
+        <v>5</v>
+      </c>
+      <c r="C260">
+        <v>380</v>
+      </c>
+      <c r="D260">
+        <v>2</v>
+      </c>
+      <c r="E260">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>14</v>
+      </c>
+      <c r="B261" t="s">
+        <v>6</v>
+      </c>
+      <c r="C261">
+        <v>380</v>
+      </c>
+      <c r="D261">
+        <v>0</v>
+      </c>
+      <c r="E261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>15</v>
+      </c>
+      <c r="B262" t="s">
+        <v>6</v>
+      </c>
+      <c r="C262">
+        <v>380</v>
+      </c>
+      <c r="D262">
+        <v>0</v>
+      </c>
+      <c r="E262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>1</v>
+      </c>
+      <c r="B263" t="s">
+        <v>5</v>
+      </c>
+      <c r="C263">
+        <v>389</v>
+      </c>
+      <c r="D263">
+        <v>1</v>
+      </c>
+      <c r="E263">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>1</v>
+      </c>
+      <c r="B264" t="s">
+        <v>6</v>
+      </c>
+      <c r="C264">
+        <v>389</v>
+      </c>
+      <c r="D264">
+        <v>0</v>
+      </c>
+      <c r="E264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>2</v>
+      </c>
+      <c r="B265" t="s">
+        <v>5</v>
+      </c>
+      <c r="C265">
+        <v>389</v>
+      </c>
+      <c r="D265">
+        <v>0</v>
+      </c>
+      <c r="E265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>2</v>
+      </c>
+      <c r="B266" t="s">
+        <v>6</v>
+      </c>
+      <c r="C266">
+        <v>389</v>
+      </c>
+      <c r="D266">
+        <v>0</v>
+      </c>
+      <c r="E266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>3</v>
+      </c>
+      <c r="B267" t="s">
+        <v>5</v>
+      </c>
+      <c r="C267">
+        <v>389</v>
+      </c>
+      <c r="D267">
+        <v>0</v>
+      </c>
+      <c r="E267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>3</v>
+      </c>
+      <c r="B268" t="s">
+        <v>6</v>
+      </c>
+      <c r="C268">
+        <v>389</v>
+      </c>
+      <c r="D268">
+        <v>0</v>
+      </c>
+      <c r="E268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>4</v>
+      </c>
+      <c r="B269" t="s">
+        <v>5</v>
+      </c>
+      <c r="C269">
+        <v>389</v>
+      </c>
+      <c r="D269">
+        <v>2</v>
+      </c>
+      <c r="E269">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>4</v>
+      </c>
+      <c r="B270" t="s">
+        <v>6</v>
+      </c>
+      <c r="C270">
+        <v>389</v>
+      </c>
+      <c r="D270">
+        <v>1</v>
+      </c>
+      <c r="E270">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>5</v>
+      </c>
+      <c r="B271" t="s">
+        <v>5</v>
+      </c>
+      <c r="C271">
+        <v>389</v>
+      </c>
+      <c r="D271">
+        <v>0</v>
+      </c>
+      <c r="E271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>5</v>
+      </c>
+      <c r="B272" t="s">
+        <v>6</v>
+      </c>
+      <c r="C272">
+        <v>389</v>
+      </c>
+      <c r="D272">
+        <v>2</v>
+      </c>
+      <c r="E272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>6</v>
+      </c>
+      <c r="B273" t="s">
+        <v>5</v>
+      </c>
+      <c r="C273">
+        <v>389</v>
+      </c>
+      <c r="D273">
+        <v>1</v>
+      </c>
+      <c r="E273">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>6</v>
+      </c>
+      <c r="B274" t="s">
+        <v>6</v>
+      </c>
+      <c r="C274">
+        <v>389</v>
+      </c>
+      <c r="D274">
+        <v>1</v>
+      </c>
+      <c r="E274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>7</v>
+      </c>
+      <c r="B275" t="s">
+        <v>5</v>
+      </c>
+      <c r="C275">
+        <v>389</v>
+      </c>
+      <c r="D275">
+        <v>0</v>
+      </c>
+      <c r="E275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>7</v>
+      </c>
+      <c r="B276" t="s">
+        <v>6</v>
+      </c>
+      <c r="C276">
+        <v>389</v>
+      </c>
+      <c r="D276">
+        <v>1</v>
+      </c>
+      <c r="E276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>8</v>
+      </c>
+      <c r="B277" t="s">
+        <v>5</v>
+      </c>
+      <c r="C277">
+        <v>389</v>
+      </c>
+      <c r="D277">
+        <v>2</v>
+      </c>
+      <c r="E277">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>8</v>
+      </c>
+      <c r="B278" t="s">
+        <v>6</v>
+      </c>
+      <c r="C278">
+        <v>389</v>
+      </c>
+      <c r="D278">
+        <v>0</v>
+      </c>
+      <c r="E278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>9</v>
+      </c>
+      <c r="B279" t="s">
+        <v>5</v>
+      </c>
+      <c r="C279">
+        <v>389</v>
+      </c>
+      <c r="D279">
+        <v>1</v>
+      </c>
+      <c r="E279">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>9</v>
+      </c>
+      <c r="B280" t="s">
+        <v>6</v>
+      </c>
+      <c r="C280">
+        <v>389</v>
+      </c>
+      <c r="D280">
+        <v>0</v>
+      </c>
+      <c r="E280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>10</v>
+      </c>
+      <c r="B281" t="s">
+        <v>5</v>
+      </c>
+      <c r="C281">
+        <v>389</v>
+      </c>
+      <c r="D281">
+        <v>1</v>
+      </c>
+      <c r="E281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>10</v>
+      </c>
+      <c r="B282" t="s">
+        <v>6</v>
+      </c>
+      <c r="C282">
+        <v>389</v>
+      </c>
+      <c r="D282">
+        <v>0</v>
+      </c>
+      <c r="E282">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>11</v>
+      </c>
+      <c r="B283" t="s">
+        <v>5</v>
+      </c>
+      <c r="C283">
+        <v>389</v>
+      </c>
+      <c r="D283">
+        <v>0</v>
+      </c>
+      <c r="E283">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>11</v>
+      </c>
+      <c r="B284" t="s">
+        <v>6</v>
+      </c>
+      <c r="C284">
+        <v>389</v>
+      </c>
+      <c r="D284">
+        <v>0</v>
+      </c>
+      <c r="E284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>12</v>
+      </c>
+      <c r="B285" t="s">
+        <v>5</v>
+      </c>
+      <c r="C285">
+        <v>389</v>
+      </c>
+      <c r="D285">
+        <v>3</v>
+      </c>
+      <c r="E285">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>12</v>
+      </c>
+      <c r="B286" t="s">
+        <v>6</v>
+      </c>
+      <c r="C286">
+        <v>389</v>
+      </c>
+      <c r="D286">
+        <v>0</v>
+      </c>
+      <c r="E286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <v>13</v>
+      </c>
+      <c r="B287" t="s">
+        <v>5</v>
+      </c>
+      <c r="C287">
+        <v>389</v>
+      </c>
+      <c r="D287">
+        <v>0</v>
+      </c>
+      <c r="E287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>13</v>
+      </c>
+      <c r="B288" t="s">
+        <v>6</v>
+      </c>
+      <c r="C288">
+        <v>389</v>
+      </c>
+      <c r="D288">
+        <v>1</v>
+      </c>
+      <c r="E288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <v>14</v>
+      </c>
+      <c r="B289" t="s">
+        <v>5</v>
+      </c>
+      <c r="C289">
+        <v>389</v>
+      </c>
+      <c r="D289">
+        <v>2</v>
+      </c>
+      <c r="E289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <v>14</v>
+      </c>
+      <c r="B290" t="s">
+        <v>6</v>
+      </c>
+      <c r="C290">
+        <v>389</v>
+      </c>
+      <c r="D290">
+        <v>0</v>
+      </c>
+      <c r="E290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <v>15</v>
+      </c>
+      <c r="B291" t="s">
+        <v>6</v>
+      </c>
+      <c r="C291">
+        <v>389</v>
+      </c>
+      <c r="D291">
+        <v>0</v>
+      </c>
+      <c r="E291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <v>1</v>
+      </c>
+      <c r="B292" t="s">
+        <v>5</v>
+      </c>
+      <c r="C292">
+        <v>404</v>
+      </c>
+      <c r="D292">
+        <v>1</v>
+      </c>
+      <c r="E292">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <v>1</v>
+      </c>
+      <c r="B293" t="s">
+        <v>6</v>
+      </c>
+      <c r="C293">
+        <v>404</v>
+      </c>
+      <c r="D293">
+        <v>0</v>
+      </c>
+      <c r="E293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>2</v>
+      </c>
+      <c r="B294" t="s">
+        <v>5</v>
+      </c>
+      <c r="C294">
+        <v>404</v>
+      </c>
+      <c r="D294">
+        <v>0</v>
+      </c>
+      <c r="E294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>2</v>
+      </c>
+      <c r="B295" t="s">
+        <v>6</v>
+      </c>
+      <c r="C295">
+        <v>404</v>
+      </c>
+      <c r="D295">
+        <v>0</v>
+      </c>
+      <c r="E295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <v>3</v>
+      </c>
+      <c r="B296" t="s">
+        <v>5</v>
+      </c>
+      <c r="C296">
+        <v>404</v>
+      </c>
+      <c r="D296">
+        <v>0</v>
+      </c>
+      <c r="E296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <v>3</v>
+      </c>
+      <c r="B297" t="s">
+        <v>6</v>
+      </c>
+      <c r="C297">
+        <v>404</v>
+      </c>
+      <c r="D297">
+        <v>0</v>
+      </c>
+      <c r="E297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A298">
+        <v>4</v>
+      </c>
+      <c r="B298" t="s">
+        <v>5</v>
+      </c>
+      <c r="C298">
+        <v>404</v>
+      </c>
+      <c r="D298">
+        <v>0</v>
+      </c>
+      <c r="E298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A299">
+        <v>4</v>
+      </c>
+      <c r="B299" t="s">
+        <v>6</v>
+      </c>
+      <c r="C299">
+        <v>404</v>
+      </c>
+      <c r="D299">
+        <v>0</v>
+      </c>
+      <c r="E299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A300">
+        <v>5</v>
+      </c>
+      <c r="B300" t="s">
+        <v>5</v>
+      </c>
+      <c r="C300">
+        <v>404</v>
+      </c>
+      <c r="D300">
+        <v>0</v>
+      </c>
+      <c r="E300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <v>5</v>
+      </c>
+      <c r="B301" t="s">
+        <v>6</v>
+      </c>
+      <c r="C301">
+        <v>404</v>
+      </c>
+      <c r="D301">
+        <v>0</v>
+      </c>
+      <c r="E301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>6</v>
+      </c>
+      <c r="B302" t="s">
+        <v>5</v>
+      </c>
+      <c r="C302">
+        <v>404</v>
+      </c>
+      <c r="D302">
+        <v>0</v>
+      </c>
+      <c r="E302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>6</v>
+      </c>
+      <c r="B303" t="s">
+        <v>6</v>
+      </c>
+      <c r="C303">
+        <v>404</v>
+      </c>
+      <c r="D303">
+        <v>0</v>
+      </c>
+      <c r="E303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <v>7</v>
+      </c>
+      <c r="B304" t="s">
+        <v>5</v>
+      </c>
+      <c r="C304">
+        <v>404</v>
+      </c>
+      <c r="D304">
+        <v>0</v>
+      </c>
+      <c r="E304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>7</v>
+      </c>
+      <c r="B305" t="s">
+        <v>6</v>
+      </c>
+      <c r="C305">
+        <v>404</v>
+      </c>
+      <c r="D305">
+        <v>0</v>
+      </c>
+      <c r="E305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>8</v>
+      </c>
+      <c r="B306" t="s">
+        <v>5</v>
+      </c>
+      <c r="C306">
+        <v>404</v>
+      </c>
+      <c r="D306">
+        <v>1</v>
+      </c>
+      <c r="E306">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>8</v>
+      </c>
+      <c r="B307" t="s">
+        <v>6</v>
+      </c>
+      <c r="C307">
+        <v>404</v>
+      </c>
+      <c r="D307">
+        <v>0</v>
+      </c>
+      <c r="E307">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>9</v>
+      </c>
+      <c r="B308" t="s">
+        <v>5</v>
+      </c>
+      <c r="C308">
+        <v>404</v>
+      </c>
+      <c r="D308">
+        <v>0</v>
+      </c>
+      <c r="E308">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>9</v>
+      </c>
+      <c r="B309" t="s">
+        <v>6</v>
+      </c>
+      <c r="C309">
+        <v>404</v>
+      </c>
+      <c r="D309">
+        <v>0</v>
+      </c>
+      <c r="E309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>10</v>
+      </c>
+      <c r="B310" t="s">
+        <v>5</v>
+      </c>
+      <c r="C310">
+        <v>404</v>
+      </c>
+      <c r="D310">
+        <v>0</v>
+      </c>
+      <c r="E310">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <v>10</v>
+      </c>
+      <c r="B311" t="s">
+        <v>6</v>
+      </c>
+      <c r="C311">
+        <v>404</v>
+      </c>
+      <c r="D311">
+        <v>1</v>
+      </c>
+      <c r="E311">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <v>11</v>
+      </c>
+      <c r="B312" t="s">
+        <v>5</v>
+      </c>
+      <c r="C312">
+        <v>404</v>
+      </c>
+      <c r="D312">
+        <v>1</v>
+      </c>
+      <c r="E312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <v>11</v>
+      </c>
+      <c r="B313" t="s">
+        <v>6</v>
+      </c>
+      <c r="C313">
+        <v>404</v>
+      </c>
+      <c r="D313">
+        <v>0</v>
+      </c>
+      <c r="E313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>12</v>
+      </c>
+      <c r="B314" t="s">
+        <v>5</v>
+      </c>
+      <c r="C314">
+        <v>404</v>
+      </c>
+      <c r="D314">
+        <v>2</v>
+      </c>
+      <c r="E314">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>12</v>
+      </c>
+      <c r="B315" t="s">
+        <v>6</v>
+      </c>
+      <c r="C315">
+        <v>404</v>
+      </c>
+      <c r="D315">
+        <v>0</v>
+      </c>
+      <c r="E315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>13</v>
+      </c>
+      <c r="B316" t="s">
+        <v>5</v>
+      </c>
+      <c r="C316">
+        <v>404</v>
+      </c>
+      <c r="D316">
+        <v>0</v>
+      </c>
+      <c r="E316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>13</v>
+      </c>
+      <c r="B317" t="s">
+        <v>6</v>
+      </c>
+      <c r="C317">
+        <v>404</v>
+      </c>
+      <c r="D317">
+        <v>0</v>
+      </c>
+      <c r="E317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <v>14</v>
+      </c>
+      <c r="B318" t="s">
+        <v>5</v>
+      </c>
+      <c r="C318">
+        <v>404</v>
+      </c>
+      <c r="D318">
+        <v>0</v>
+      </c>
+      <c r="E318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <v>14</v>
+      </c>
+      <c r="B319" t="s">
+        <v>6</v>
+      </c>
+      <c r="C319">
+        <v>404</v>
+      </c>
+      <c r="D319">
+        <v>0</v>
+      </c>
+      <c r="E319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <v>15</v>
+      </c>
+      <c r="B320" t="s">
+        <v>6</v>
+      </c>
+      <c r="C320">
+        <v>404</v>
+      </c>
+      <c r="D320">
+        <v>0</v>
+      </c>
+      <c r="E320">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating the MFE flies data file.
</commit_message>
<xml_diff>
--- a/data/fitness_development/MFE_flies.xlsx
+++ b/data/fitness_development/MFE_flies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_19/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF6B70DB-F89E-1041-ABAD-3D5F559AAE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEBD6717-8491-9549-907A-7E4639F7AB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{F87DAE63-E76D-134A-8567-557F4C2DF883}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="10">
   <si>
     <t>vial</t>
   </si>
@@ -437,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E795774-325B-7540-93CB-61EC9638DF3F}">
-  <dimension ref="A1:F378"/>
+  <dimension ref="A1:F407"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I375" sqref="I375"/>
+    <sheetView tabSelected="1" topLeftCell="A393" zoomScale="194" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F403" sqref="F403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8008,6 +8008,586 @@
         <v>8</v>
       </c>
     </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A379">
+        <v>1</v>
+      </c>
+      <c r="B379" t="s">
+        <v>5</v>
+      </c>
+      <c r="C379">
+        <v>434</v>
+      </c>
+      <c r="D379">
+        <v>0</v>
+      </c>
+      <c r="E379">
+        <v>1</v>
+      </c>
+      <c r="F379" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A380">
+        <v>1</v>
+      </c>
+      <c r="B380" t="s">
+        <v>6</v>
+      </c>
+      <c r="C380">
+        <v>434</v>
+      </c>
+      <c r="D380">
+        <v>0</v>
+      </c>
+      <c r="E380">
+        <v>0</v>
+      </c>
+      <c r="F380" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A381">
+        <v>2</v>
+      </c>
+      <c r="B381" t="s">
+        <v>5</v>
+      </c>
+      <c r="C381">
+        <v>434</v>
+      </c>
+      <c r="D381">
+        <v>0</v>
+      </c>
+      <c r="E381">
+        <v>1</v>
+      </c>
+      <c r="F381" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A382">
+        <v>2</v>
+      </c>
+      <c r="B382" t="s">
+        <v>6</v>
+      </c>
+      <c r="C382">
+        <v>434</v>
+      </c>
+      <c r="D382">
+        <v>0</v>
+      </c>
+      <c r="E382">
+        <v>0</v>
+      </c>
+      <c r="F382" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A383">
+        <v>3</v>
+      </c>
+      <c r="B383" t="s">
+        <v>5</v>
+      </c>
+      <c r="C383">
+        <v>434</v>
+      </c>
+      <c r="D383">
+        <v>0</v>
+      </c>
+      <c r="E383">
+        <v>0</v>
+      </c>
+      <c r="F383" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A384">
+        <v>3</v>
+      </c>
+      <c r="B384" t="s">
+        <v>6</v>
+      </c>
+      <c r="C384">
+        <v>434</v>
+      </c>
+      <c r="D384">
+        <v>0</v>
+      </c>
+      <c r="E384">
+        <v>0</v>
+      </c>
+      <c r="F384" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A385">
+        <v>4</v>
+      </c>
+      <c r="B385" t="s">
+        <v>5</v>
+      </c>
+      <c r="C385">
+        <v>434</v>
+      </c>
+      <c r="D385">
+        <v>0</v>
+      </c>
+      <c r="E385">
+        <v>1</v>
+      </c>
+      <c r="F385" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A386">
+        <v>4</v>
+      </c>
+      <c r="B386" t="s">
+        <v>6</v>
+      </c>
+      <c r="C386">
+        <v>434</v>
+      </c>
+      <c r="D386">
+        <v>0</v>
+      </c>
+      <c r="E386">
+        <v>0</v>
+      </c>
+      <c r="F386" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A387">
+        <v>5</v>
+      </c>
+      <c r="B387" t="s">
+        <v>5</v>
+      </c>
+      <c r="C387">
+        <v>434</v>
+      </c>
+      <c r="D387">
+        <v>0</v>
+      </c>
+      <c r="E387">
+        <v>0</v>
+      </c>
+      <c r="F387" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A388">
+        <v>5</v>
+      </c>
+      <c r="B388" t="s">
+        <v>6</v>
+      </c>
+      <c r="C388">
+        <v>434</v>
+      </c>
+      <c r="D388">
+        <v>0</v>
+      </c>
+      <c r="E388">
+        <v>0</v>
+      </c>
+      <c r="F388" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A389">
+        <v>6</v>
+      </c>
+      <c r="B389" t="s">
+        <v>5</v>
+      </c>
+      <c r="C389">
+        <v>434</v>
+      </c>
+      <c r="D389">
+        <v>0</v>
+      </c>
+      <c r="E389">
+        <v>0</v>
+      </c>
+      <c r="F389" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A390">
+        <v>6</v>
+      </c>
+      <c r="B390" t="s">
+        <v>6</v>
+      </c>
+      <c r="C390">
+        <v>434</v>
+      </c>
+      <c r="D390">
+        <v>0</v>
+      </c>
+      <c r="E390">
+        <v>0</v>
+      </c>
+      <c r="F390" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A391">
+        <v>7</v>
+      </c>
+      <c r="B391" t="s">
+        <v>5</v>
+      </c>
+      <c r="C391">
+        <v>434</v>
+      </c>
+      <c r="D391">
+        <v>0</v>
+      </c>
+      <c r="E391">
+        <v>0</v>
+      </c>
+      <c r="F391" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A392">
+        <v>7</v>
+      </c>
+      <c r="B392" t="s">
+        <v>6</v>
+      </c>
+      <c r="C392">
+        <v>434</v>
+      </c>
+      <c r="D392">
+        <v>0</v>
+      </c>
+      <c r="E392">
+        <v>0</v>
+      </c>
+      <c r="F392" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A393">
+        <v>8</v>
+      </c>
+      <c r="B393" t="s">
+        <v>5</v>
+      </c>
+      <c r="C393">
+        <v>434</v>
+      </c>
+      <c r="D393">
+        <v>0</v>
+      </c>
+      <c r="E393">
+        <v>0</v>
+      </c>
+      <c r="F393" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A394">
+        <v>8</v>
+      </c>
+      <c r="B394" t="s">
+        <v>6</v>
+      </c>
+      <c r="C394">
+        <v>434</v>
+      </c>
+      <c r="D394">
+        <v>0</v>
+      </c>
+      <c r="E394">
+        <v>0</v>
+      </c>
+      <c r="F394" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A395">
+        <v>9</v>
+      </c>
+      <c r="B395" t="s">
+        <v>5</v>
+      </c>
+      <c r="C395">
+        <v>434</v>
+      </c>
+      <c r="D395">
+        <v>0</v>
+      </c>
+      <c r="E395">
+        <v>2</v>
+      </c>
+      <c r="F395" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A396">
+        <v>9</v>
+      </c>
+      <c r="B396" t="s">
+        <v>6</v>
+      </c>
+      <c r="C396">
+        <v>434</v>
+      </c>
+      <c r="D396">
+        <v>0</v>
+      </c>
+      <c r="E396">
+        <v>0</v>
+      </c>
+      <c r="F396" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A397">
+        <v>10</v>
+      </c>
+      <c r="B397" t="s">
+        <v>5</v>
+      </c>
+      <c r="C397">
+        <v>434</v>
+      </c>
+      <c r="D397">
+        <v>0</v>
+      </c>
+      <c r="E397">
+        <v>0</v>
+      </c>
+      <c r="F397" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A398">
+        <v>10</v>
+      </c>
+      <c r="B398" t="s">
+        <v>6</v>
+      </c>
+      <c r="C398">
+        <v>434</v>
+      </c>
+      <c r="D398">
+        <v>0</v>
+      </c>
+      <c r="E398">
+        <v>0</v>
+      </c>
+      <c r="F398" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A399">
+        <v>11</v>
+      </c>
+      <c r="B399" t="s">
+        <v>5</v>
+      </c>
+      <c r="C399">
+        <v>434</v>
+      </c>
+      <c r="D399">
+        <v>0</v>
+      </c>
+      <c r="E399">
+        <v>0</v>
+      </c>
+      <c r="F399" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A400">
+        <v>11</v>
+      </c>
+      <c r="B400" t="s">
+        <v>6</v>
+      </c>
+      <c r="C400">
+        <v>434</v>
+      </c>
+      <c r="D400">
+        <v>0</v>
+      </c>
+      <c r="E400">
+        <v>1</v>
+      </c>
+      <c r="F400" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A401">
+        <v>12</v>
+      </c>
+      <c r="B401" t="s">
+        <v>5</v>
+      </c>
+      <c r="C401">
+        <v>434</v>
+      </c>
+      <c r="D401">
+        <v>0</v>
+      </c>
+      <c r="E401">
+        <v>0</v>
+      </c>
+      <c r="F401" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A402">
+        <v>12</v>
+      </c>
+      <c r="B402" t="s">
+        <v>6</v>
+      </c>
+      <c r="C402">
+        <v>434</v>
+      </c>
+      <c r="D402">
+        <v>0</v>
+      </c>
+      <c r="E402">
+        <v>0</v>
+      </c>
+      <c r="F402" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A403">
+        <v>13</v>
+      </c>
+      <c r="B403" t="s">
+        <v>5</v>
+      </c>
+      <c r="C403">
+        <v>434</v>
+      </c>
+      <c r="D403">
+        <v>0</v>
+      </c>
+      <c r="E403">
+        <v>0</v>
+      </c>
+      <c r="F403" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A404">
+        <v>13</v>
+      </c>
+      <c r="B404" t="s">
+        <v>6</v>
+      </c>
+      <c r="C404">
+        <v>434</v>
+      </c>
+      <c r="D404">
+        <v>0</v>
+      </c>
+      <c r="E404">
+        <v>0</v>
+      </c>
+      <c r="F404" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A405">
+        <v>14</v>
+      </c>
+      <c r="B405" t="s">
+        <v>5</v>
+      </c>
+      <c r="C405">
+        <v>434</v>
+      </c>
+      <c r="D405">
+        <v>0</v>
+      </c>
+      <c r="E405">
+        <v>0</v>
+      </c>
+      <c r="F405" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A406">
+        <v>14</v>
+      </c>
+      <c r="B406" t="s">
+        <v>6</v>
+      </c>
+      <c r="C406">
+        <v>434</v>
+      </c>
+      <c r="D406">
+        <v>0</v>
+      </c>
+      <c r="E406">
+        <v>0</v>
+      </c>
+      <c r="F406" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A407">
+        <v>15</v>
+      </c>
+      <c r="B407" t="s">
+        <v>6</v>
+      </c>
+      <c r="C407">
+        <v>434</v>
+      </c>
+      <c r="D407">
+        <v>0</v>
+      </c>
+      <c r="E407">
+        <v>0</v>
+      </c>
+      <c r="F407" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>